<commit_message>
Finished quest scraping, started equipment scraping and edited monster scraping
</commit_message>
<xml_diff>
--- a/osrs_quests.xlsx
+++ b/osrs_quests.xlsx
@@ -6081,17 +6081,19 @@
           <t>Medium</t>
         </is>
       </c>
-      <c r="D177" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="D177" t="n">
+        <v>0</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F177" t="inlineStr">
+        <is>
           <t>25 March 2002</t>
         </is>
       </c>
-      <c r="F177" t="inlineStr"/>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -6109,17 +6111,19 @@
           <t>Medium</t>
         </is>
       </c>
-      <c r="D178" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="D178" t="n">
+        <v>0</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F178" t="inlineStr">
+        <is>
           <t>3 July 2007</t>
         </is>
       </c>
-      <c r="F178" t="inlineStr"/>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -6137,17 +6141,19 @@
           <t>Short</t>
         </is>
       </c>
-      <c r="D179" t="inlineStr">
+      <c r="D179" t="n">
+        <v>0</v>
+      </c>
+      <c r="E179" t="inlineStr">
         <is>
           <t>Great Kourend</t>
         </is>
       </c>
-      <c r="E179" t="inlineStr">
+      <c r="F179" t="inlineStr">
         <is>
           <t>19 May 2016</t>
         </is>
       </c>
-      <c r="F179" t="inlineStr"/>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -6165,17 +6171,19 @@
           <t>Medium</t>
         </is>
       </c>
-      <c r="D180" t="inlineStr">
+      <c r="D180" t="n">
+        <v>0</v>
+      </c>
+      <c r="E180" t="inlineStr">
         <is>
           <t>Mahjarrat, #8</t>
         </is>
       </c>
-      <c r="E180" t="inlineStr">
+      <c r="F180" t="inlineStr">
         <is>
           <t>26 July 2005</t>
         </is>
       </c>
-      <c r="F180" t="inlineStr"/>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -6193,17 +6201,19 @@
           <t>Short</t>
         </is>
       </c>
-      <c r="D181" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="D181" t="n">
+        <v>0</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F181" t="inlineStr">
+        <is>
           <t>26 August 2020</t>
         </is>
       </c>
-      <c r="F181" t="inlineStr"/>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -6221,17 +6231,19 @@
           <t>Medium</t>
         </is>
       </c>
-      <c r="D182" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="D182" t="n">
+        <v>0</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F182" t="inlineStr">
+        <is>
           <t>22 November 2005</t>
         </is>
       </c>
-      <c r="F182" t="inlineStr"/>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -6249,17 +6261,19 @@
           <t>Very Short</t>
         </is>
       </c>
-      <c r="D183" t="inlineStr">
+      <c r="D183" t="n">
+        <v>0</v>
+      </c>
+      <c r="E183" t="inlineStr">
         <is>
           <t>Order of Wizards, #2</t>
         </is>
       </c>
-      <c r="E183" t="inlineStr">
+      <c r="F183" t="inlineStr">
         <is>
           <t>13 June 2005</t>
         </is>
       </c>
-      <c r="F183" t="inlineStr"/>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -6277,17 +6291,19 @@
           <t>Short</t>
         </is>
       </c>
-      <c r="D184" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="D184" t="n">
+        <v>0</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F184" t="inlineStr">
+        <is>
           <t>1 September 2016</t>
         </is>
       </c>
-      <c r="F184" t="inlineStr"/>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -6305,17 +6321,19 @@
           <t>Short</t>
         </is>
       </c>
-      <c r="D185" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="D185" t="n">
+        <v>0</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F185" t="inlineStr">
+        <is>
           <t>16 December 2021</t>
         </is>
       </c>
-      <c r="F185" t="inlineStr"/>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -6333,17 +6351,19 @@
           <t>Medium</t>
         </is>
       </c>
-      <c r="D186" t="inlineStr">
+      <c r="D186" t="n">
+        <v>0</v>
+      </c>
+      <c r="E186" t="inlineStr">
         <is>
           <t>Mahjarrat, #9</t>
         </is>
       </c>
-      <c r="E186" t="inlineStr">
+      <c r="F186" t="inlineStr">
         <is>
           <t>12 February 2007</t>
         </is>
       </c>
-      <c r="F186" t="inlineStr"/>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
@@ -6361,17 +6381,19 @@
           <t>Short</t>
         </is>
       </c>
-      <c r="D187" t="inlineStr">
+      <c r="D187" t="n">
+        <v>0</v>
+      </c>
+      <c r="E187" t="inlineStr">
         <is>
           <t>Mahjarrat, #11</t>
         </is>
       </c>
-      <c r="E187" t="inlineStr">
+      <c r="F187" t="inlineStr">
         <is>
           <t>14 June 2023</t>
         </is>
       </c>
-      <c r="F187" t="inlineStr"/>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
@@ -6389,17 +6411,19 @@
           <t>Short</t>
         </is>
       </c>
-      <c r="D188" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="D188" t="n">
+        <v>0</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F188" t="inlineStr">
+        <is>
           <t>9 February 2022</t>
         </is>
       </c>
-      <c r="F188" t="inlineStr"/>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -6417,17 +6441,19 @@
           <t>Medium</t>
         </is>
       </c>
-      <c r="D189" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="D189" t="n">
+        <v>0</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F189" t="inlineStr">
+        <is>
           <t>4 July 2019</t>
         </is>
       </c>
-      <c r="F189" t="inlineStr"/>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
@@ -6445,17 +6471,19 @@
           <t>Medium</t>
         </is>
       </c>
-      <c r="D190" t="inlineStr">
+      <c r="D190" t="n">
+        <v>0</v>
+      </c>
+      <c r="E190" t="inlineStr">
         <is>
           <t>Kharidian, #5</t>
         </is>
       </c>
-      <c r="E190" t="inlineStr">
+      <c r="F190" t="inlineStr">
         <is>
           <t>24 August 2022</t>
         </is>
       </c>
-      <c r="F190" t="inlineStr"/>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -6473,17 +6501,19 @@
           <t>Medium</t>
         </is>
       </c>
-      <c r="D191" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="D191" t="n">
+        <v>0</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F191" t="inlineStr">
+        <is>
           <t>22 January 2007</t>
         </is>
       </c>
-      <c r="F191" t="inlineStr"/>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -6501,17 +6531,19 @@
           <t>Short</t>
         </is>
       </c>
-      <c r="D192" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="D192" t="n">
+        <v>0</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F192" t="inlineStr">
+        <is>
           <t>22 September 2003</t>
         </is>
       </c>
-      <c r="F192" t="inlineStr"/>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
@@ -6529,17 +6561,19 @@
           <t>Medium</t>
         </is>
       </c>
-      <c r="D193" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="D193" t="n">
+        <v>0</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F193" t="inlineStr">
+        <is>
           <t>23 November 2017</t>
         </is>
       </c>
-      <c r="F193" t="inlineStr"/>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
@@ -6557,17 +6591,19 @@
           <t>Very Short</t>
         </is>
       </c>
-      <c r="D194" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="D194" t="n">
+        <v>0</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F194" t="inlineStr">
+        <is>
           <t>24 October 2005</t>
         </is>
       </c>
-      <c r="F194" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>